<commit_message>
Updating project plan with current effort's status.
</commit_message>
<xml_diff>
--- a/gantt_chart_project_plan.xlsx
+++ b/gantt_chart_project_plan.xlsx
@@ -1,51 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielklass/Dropbox/GaTech/cse6242_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CD38A-84AA-A243-B2B4-A4149E4CAB7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FADB0EB-3899-7A44-AED4-B0859D03F96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="440" windowWidth="24840" windowHeight="28360" activeTab="1" xr2:uid="{7361172A-1EC7-8B42-8F6F-CEFE35A9BD9E}"/>
+    <workbookView xWindow="1600" yWindow="440" windowWidth="24840" windowHeight="28360" xr2:uid="{7361172A-1EC7-8B42-8F6F-CEFE35A9BD9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Jon's Recommendations" sheetId="4" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$32</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$G$2:$G$32</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$2:$A$32</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t>Done</t>
   </si>
@@ -280,6 +251,9 @@
   </si>
   <si>
     <t>Write final report and poster</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -287,8 +261,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="167" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -328,9 +302,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1005,7 +979,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2025,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463EE16C-606B-984A-A884-7D08EC404BBB}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScale="133" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2223,6 +2197,9 @@
       <c r="A8" t="s">
         <v>29</v>
       </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
       <c r="C8" s="1">
         <v>43728</v>
       </c>
@@ -2246,6 +2223,9 @@
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
       <c r="C9" s="1">
         <v>43728</v>
       </c>
@@ -2269,6 +2249,9 @@
       <c r="A10" t="s">
         <v>26</v>
       </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
       <c r="C10" s="1">
         <v>43728</v>
       </c>
@@ -2292,6 +2275,9 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
       <c r="C11" s="1">
         <v>43728</v>
       </c>
@@ -2315,6 +2301,9 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
       <c r="C12" s="1">
         <v>43728</v>
       </c>
@@ -2338,6 +2327,9 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
       <c r="C13" s="1">
         <v>43728</v>
       </c>
@@ -2361,7 +2353,9 @@
       <c r="A14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="C14" s="6">
         <v>43749</v>
       </c>
@@ -2386,7 +2380,9 @@
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="C15" s="6">
         <v>43749</v>
       </c>
@@ -2411,7 +2407,9 @@
       <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="C16" s="6">
         <v>43751</v>
       </c>
@@ -2438,6 +2436,9 @@
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
       <c r="C17" s="1">
         <v>43749</v>
       </c>
@@ -2461,7 +2462,9 @@
       <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B18"/>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
       <c r="C18" s="1">
         <v>43749</v>
       </c>
@@ -2488,7 +2491,9 @@
       <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B19"/>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
       <c r="C19" s="1">
         <v>43749</v>
       </c>
@@ -2515,7 +2520,9 @@
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
       <c r="C20" s="1">
         <v>43758</v>
       </c>
@@ -2540,7 +2547,9 @@
       <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B21"/>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
       <c r="C21" s="1">
         <v>43758</v>
       </c>
@@ -2565,7 +2574,9 @@
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22"/>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
       <c r="C22" s="1">
         <v>43768</v>
       </c>
@@ -2592,7 +2603,9 @@
       <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B23"/>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
       <c r="C23" s="1">
         <v>43768</v>
       </c>
@@ -2617,7 +2630,9 @@
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
       <c r="C24" s="1">
         <v>43749</v>
       </c>
@@ -2845,12 +2860,12 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="9">
         <f ca="1">TODAY()+5/24-18/24</f>
-        <v>43742.458333333336</v>
+        <v>43763.458333333336</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="8">
         <f ca="1">NOW()+13.5/24</f>
-        <v>43744.374408449075</v>
+        <v>43765.106666435182</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2860,7 +2875,7 @@
       </c>
       <c r="B35" s="9">
         <f ca="1">NOW()+13.75/24</f>
-        <v>43744.38482511574</v>
+        <v>43765.117083101846</v>
       </c>
       <c r="C35" s="10"/>
     </row>
@@ -2877,7 +2892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC1758F-7DFD-1C4B-AA11-E6F3F5750601}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating task data a bit.
</commit_message>
<xml_diff>
--- a/gantt_chart_project_plan.xlsx
+++ b/gantt_chart_project_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielklass/Dropbox/GaTech/cse6242_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FADB0EB-3899-7A44-AED4-B0859D03F96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1AE66E-2E51-2F4E-8480-DE79A06F07BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="440" windowWidth="24840" windowHeight="28360" xr2:uid="{7361172A-1EC7-8B42-8F6F-CEFE35A9BD9E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>Done</t>
   </si>
@@ -73,15 +73,6 @@
     <t>Start_Date_DateFormat</t>
   </si>
   <si>
-    <t>&gt;Slides: Rocko</t>
-  </si>
-  <si>
-    <t>&gt;Video: Daniel</t>
-  </si>
-  <si>
-    <t>&gt;Paper: All</t>
-  </si>
-  <si>
     <t>Experimental Coding (Daniel, Yi: Done)</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t>==========Progress Report (All)==========</t>
   </si>
   <si>
-    <t>&gt;LaTeX Compile &amp; Submission: Rocko</t>
-  </si>
-  <si>
     <t>============Algorithm Polish============</t>
   </si>
   <si>
@@ -142,30 +130,12 @@
     <t>&gt;Plot projected movies (All)</t>
   </si>
   <si>
-    <t>&gt;Embed Movies in Taste Space</t>
-  </si>
-  <si>
-    <t>&gt;Implement TSNE (Rocko, Jonathan)</t>
-  </si>
-  <si>
-    <t>&gt;Pre-cluster movies (Rocko, Jonathan)</t>
-  </si>
-  <si>
-    <t>&gt;Understand MovieExplorer Code/Algo</t>
-  </si>
-  <si>
     <t>&gt;Implement Exploration Code (no UI) (Yi, Rocko)</t>
   </si>
   <si>
     <t>=======Implement MovieExplorer========</t>
   </si>
   <si>
-    <t>&gt;Implement Matrix Factor Algo (Jonathan)</t>
-  </si>
-  <si>
-    <t>&gt;Implement Word2Vec Algo (Daniel, Yi)</t>
-  </si>
-  <si>
     <t>&gt;GUI initial build (All)</t>
   </si>
   <si>
@@ -254,6 +224,36 @@
   </si>
   <si>
     <t>WIP</t>
+  </si>
+  <si>
+    <t>&gt;Understand MovieExplorer Code/Algo (All: Done)</t>
+  </si>
+  <si>
+    <t>&gt;LaTeX Compile &amp; Submission (Rocko: Done)</t>
+  </si>
+  <si>
+    <t>&gt;Paper (All, Done)</t>
+  </si>
+  <si>
+    <t>&gt;Slides (Rocko: Done)</t>
+  </si>
+  <si>
+    <t>&gt;Video (Daniel: Done)</t>
+  </si>
+  <si>
+    <t>&gt;Implement Matrix Factor Algo (Jonathan: Done)</t>
+  </si>
+  <si>
+    <t>&gt;Implement Word2Vec Algo (Daniel, Yi: Done)</t>
+  </si>
+  <si>
+    <t>&gt;Embed Movies in Taste Space (Daniel: Done)</t>
+  </si>
+  <si>
+    <t>&gt;Implement TSNE (Rocko, Jonathan, Daniel: Done)</t>
+  </si>
+  <si>
+    <t>&gt;Pre-cluster movies (Rocko, Jonathan, Daniel: Done)</t>
   </si>
 </sst>
 </file>
@@ -466,22 +466,22 @@
                   <c:v>========Project Proposal Due (All)========</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>&gt;LaTeX Compile &amp; Submission: Rocko</c:v>
+                  <c:v>&gt;LaTeX Compile &amp; Submission (Rocko: Done)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>&gt;Paper: All</c:v>
+                  <c:v>&gt;Paper (All, Done)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>&gt;Slides: Rocko</c:v>
+                  <c:v>&gt;Slides (Rocko: Done)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>&gt;Video: Daniel</c:v>
+                  <c:v>&gt;Video (Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>=======Implement MovieExplorer========</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>&gt;Understand MovieExplorer Code/Algo</c:v>
+                  <c:v>&gt;Understand MovieExplorer Code/Algo (All: Done)</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>&gt;Implement Exploration Code (no UI) (Yi, Rocko)</c:v>
@@ -490,22 +490,22 @@
                   <c:v>======Collaborative Filtering Engine======</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>&gt;Implement Matrix Factor Algo (Jonathan)</c:v>
+                  <c:v>&gt;Implement Matrix Factor Algo (Jonathan: Done)</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>&gt;Implement Word2Vec Algo (Daniel, Yi)</c:v>
+                  <c:v>&gt;Implement Word2Vec Algo (Daniel, Yi: Done)</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>=======Visualization Preprocessing=======</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>&gt;Embed Movies in Taste Space</c:v>
+                  <c:v>&gt;Embed Movies in Taste Space (Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>&gt;Implement TSNE (Rocko, Jonathan)</c:v>
+                  <c:v>&gt;Implement TSNE (Rocko, Jonathan, Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>&gt;Pre-cluster movies (Rocko, Jonathan)</c:v>
+                  <c:v>&gt;Pre-cluster movies (Rocko, Jonathan, Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>==========Progress Report (All)==========</c:v>
@@ -701,22 +701,22 @@
                   <c:v>========Project Proposal Due (All)========</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>&gt;LaTeX Compile &amp; Submission: Rocko</c:v>
+                  <c:v>&gt;LaTeX Compile &amp; Submission (Rocko: Done)</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>&gt;Paper: All</c:v>
+                  <c:v>&gt;Paper (All, Done)</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>&gt;Slides: Rocko</c:v>
+                  <c:v>&gt;Slides (Rocko: Done)</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>&gt;Video: Daniel</c:v>
+                  <c:v>&gt;Video (Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>=======Implement MovieExplorer========</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>&gt;Understand MovieExplorer Code/Algo</c:v>
+                  <c:v>&gt;Understand MovieExplorer Code/Algo (All: Done)</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>&gt;Implement Exploration Code (no UI) (Yi, Rocko)</c:v>
@@ -725,22 +725,22 @@
                   <c:v>======Collaborative Filtering Engine======</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>&gt;Implement Matrix Factor Algo (Jonathan)</c:v>
+                  <c:v>&gt;Implement Matrix Factor Algo (Jonathan: Done)</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>&gt;Implement Word2Vec Algo (Daniel, Yi)</c:v>
+                  <c:v>&gt;Implement Word2Vec Algo (Daniel, Yi: Done)</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>=======Visualization Preprocessing=======</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>&gt;Embed Movies in Taste Space</c:v>
+                  <c:v>&gt;Embed Movies in Taste Space (Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>&gt;Implement TSNE (Rocko, Jonathan)</c:v>
+                  <c:v>&gt;Implement TSNE (Rocko, Jonathan, Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>&gt;Pre-cluster movies (Rocko, Jonathan)</c:v>
+                  <c:v>&gt;Pre-cluster movies (Rocko, Jonathan, Daniel: Done)</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>==========Progress Report (All)==========</c:v>
@@ -2000,12 +2000,12 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" style="2"/>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2065,7 +2065,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>0</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>0</v>
@@ -2434,7 +2434,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -2518,10 +2518,10 @@
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1">
         <v>43758</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -2601,10 +2601,10 @@
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C23" s="1">
         <v>43768</v>
@@ -2628,10 +2628,10 @@
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C24" s="1">
         <v>43749</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1">
         <v>43777</v>
@@ -2683,7 +2683,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
       </c>
       <c r="C26" s="1">
         <v>43777</v>
@@ -2706,7 +2709,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
       </c>
       <c r="C27" s="1">
         <v>43777</v>
@@ -2729,7 +2735,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
       </c>
       <c r="C28" s="1">
         <v>43784</v>
@@ -2752,7 +2761,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1">
         <v>43784</v>
@@ -2778,7 +2787,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1">
         <v>43784</v>
@@ -2804,7 +2813,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1">
         <v>43784</v>
@@ -2830,7 +2839,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C32" s="1">
         <v>43784</v>
@@ -2865,7 +2874,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="8">
         <f ca="1">NOW()+13.5/24</f>
-        <v>43765.106666435182</v>
+        <v>43765.110000347224</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2875,7 +2884,7 @@
       </c>
       <c r="B35" s="9">
         <f ca="1">NOW()+13.75/24</f>
-        <v>43765.117083101846</v>
+        <v>43765.120417013888</v>
       </c>
       <c r="C35" s="10"/>
     </row>
@@ -2905,21 +2914,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
         <v>43751</v>
@@ -2927,10 +2936,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1">
         <v>43754</v>
@@ -2938,15 +2947,15 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1">
         <v>43758</v>
@@ -2954,10 +2963,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1">
         <v>43758</v>
@@ -2965,15 +2974,15 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1">
         <v>43751</v>
@@ -2981,10 +2990,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1">
         <v>43761</v>
@@ -2992,15 +3001,15 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1">
         <v>43768</v>
@@ -3008,10 +3017,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1">
         <v>43772</v>
@@ -3019,10 +3028,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1">
         <v>43772</v>
@@ -3035,10 +3044,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1">
         <v>43777</v>
@@ -3046,15 +3055,15 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1">
         <v>43784</v>
@@ -3062,10 +3071,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1">
         <v>43791</v>
@@ -3073,10 +3082,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1">
         <v>43798</v>
@@ -3089,10 +3098,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1">
         <v>43798</v>

</xml_diff>